<commit_message>
Excel custom header example output
</commit_message>
<xml_diff>
--- a/example_file/output_with_header.xlsx
+++ b/example_file/output_with_header.xlsx
@@ -14,7 +14,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+  <x:si>
+    <x:t>Id</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Age</x:t>
+  </x:si>
   <x:si>
     <x:t>John</x:t>
   </x:si>
@@ -149,12 +158,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C24" totalsRowShown="0">
-  <x:autoFilter ref="A1:C24"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C25" totalsRowShown="0">
+  <x:autoFilter ref="A1:C25"/>
   <x:tableColumns count="3">
-    <x:tableColumn id="1" name="1"/>
-    <x:tableColumn id="2" name="John"/>
-    <x:tableColumn id="3" name="26"/>
+    <x:tableColumn id="1" name="Id"/>
+    <x:tableColumn id="2" name="Name"/>
+    <x:tableColumn id="3" name="Age"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
@@ -448,274 +457,285 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C24"/>
+  <x:dimension ref="A1:C25"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
     <x:row r="1" spans="1:3">
-      <x:c r="A1" s="0" t="n">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B1" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="C1" s="0" t="n">
-        <x:v>26</x:v>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:3">
       <x:c r="A2" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>1</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="C2" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:3">
       <x:c r="A3" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="C3" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:3">
       <x:c r="A4" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C4" s="0" t="n">
-        <x:v>20</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:3">
       <x:c r="A5" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C5" s="0" t="n">
-        <x:v>19</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:3">
       <x:c r="A6" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C6" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:3">
       <x:c r="A7" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C7" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:3">
       <x:c r="A8" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C8" s="0" t="n">
-        <x:v>18</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:3">
       <x:c r="A9" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C9" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:3">
       <x:c r="A10" s="0" t="n">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C10" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:3">
       <x:c r="A11" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="C11" s="0" t="n">
-        <x:v>33</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:3">
       <x:c r="A12" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C12" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:3">
       <x:c r="A13" s="0" t="n">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C13" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:3">
       <x:c r="A14" s="0" t="n">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C14" s="0" t="n">
-        <x:v>28</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:3">
       <x:c r="A15" s="0" t="n">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C15" s="0" t="n">
-        <x:v>21</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:3">
       <x:c r="A16" s="0" t="n">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C16" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:3">
       <x:c r="A17" s="0" t="n">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C17" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:3">
       <x:c r="A18" s="0" t="n">
-        <x:v>18</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C18" s="0" t="n">
-        <x:v>27</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:3">
       <x:c r="A19" s="0" t="n">
-        <x:v>19</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C19" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:3">
       <x:c r="A20" s="0" t="n">
-        <x:v>20</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C20" s="0" t="n">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:3">
       <x:c r="A21" s="0" t="n">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C21" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:3">
       <x:c r="A22" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C22" s="0" t="n">
-        <x:v>34</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:3">
       <x:c r="A23" s="0" t="n">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="n">
         <x:v>23</x:v>
-      </x:c>
-      <x:c r="B23" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="C23" s="0" t="n">
-        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:3">
       <x:c r="A24" s="0" t="n">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="n">
+        <x:v>28</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:3">
+      <x:c r="A25" s="0" t="n">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="B24" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="C24" s="0" t="n">
-        <x:v>24</x:v>
+      <x:c r="B25" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="n">
+        <x:v>22</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>